<commit_message>
Cleaned up results folder
</commit_message>
<xml_diff>
--- a/src/results/experiment1_results.xlsx
+++ b/src/results/experiment1_results.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bierce/Documents/classes/ds4300-practical-02/src/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1ED83B88-1E1F-3643-89D3-BF53874A46E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCD1703-24D3-4C40-99D2-5130A7DB366A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{45693F41-EAD8-4644-A5DD-AB9A2A698043}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{45693F41-EAD8-4644-A5DD-AB9A2A698043}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment1_results" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">experiment1_results!$A$1:$E$37</definedName>
@@ -413,16 +412,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -797,14 +789,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5754D876-32E3-5145-A84C-FAFF84FD8A1B}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="176.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="176.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
@@ -814,7 +806,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -828,10 +820,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2">
@@ -844,11 +836,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3">
@@ -862,10 +854,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4">
@@ -879,10 +871,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="372" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5">
@@ -896,10 +888,10 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C6">
@@ -912,11 +904,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="1:5" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C7">
@@ -930,10 +922,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="119" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C8">
@@ -946,11 +938,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="1:5" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C9">
@@ -964,10 +956,10 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C10">
@@ -980,11 +972,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:5" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C11">
@@ -998,10 +990,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C12">
@@ -1014,11 +1006,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="4" t="s">
+    <row r="13" spans="1:5" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C13">
@@ -1031,11 +1023,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C14">
@@ -1048,11 +1040,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:5" ht="404" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C15">
@@ -1065,11 +1057,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C16">
@@ -1082,11 +1074,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="356" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="1:5" ht="272" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C17">
@@ -1099,11 +1091,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="4" t="s">
+    <row r="18" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C18">
@@ -1116,11 +1108,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="4" t="s">
+    <row r="19" spans="1:5" ht="272" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C19">
@@ -1133,11 +1125,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="4" t="s">
+    <row r="20" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C20">
@@ -1150,11 +1142,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="323" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="4" t="s">
+    <row r="21" spans="1:5" ht="221" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C21">
@@ -1167,11 +1159,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="4" t="s">
+    <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C22">
@@ -1184,11 +1176,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="4" t="s">
+    <row r="23" spans="1:5" ht="306" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C23">
@@ -1201,11 +1193,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="4" t="s">
+    <row r="24" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C24">
@@ -1218,11 +1210,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="4" t="s">
+    <row r="25" spans="1:5" ht="340" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C25">
@@ -1235,11 +1227,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="4" t="s">
+    <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C26">
@@ -1252,11 +1244,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="272" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="4" t="s">
+    <row r="27" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C27">
@@ -1269,11 +1261,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="4" t="s">
+    <row r="28" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C28">
@@ -1286,11 +1278,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="4" t="s">
+    <row r="29" spans="1:5" ht="323" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C29">
@@ -1303,11 +1295,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="4" t="s">
+    <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C30">
@@ -1321,10 +1313,10 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="4" t="s">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C31">
@@ -1337,11 +1329,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="4" t="s">
+    <row r="32" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C32">
@@ -1354,11 +1346,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="4" t="s">
+    <row r="33" spans="1:5" ht="404" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C33">
@@ -1371,11 +1363,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="4" t="s">
+    <row r="34" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C34">
@@ -1388,11 +1380,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="306" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="4" t="s">
+    <row r="35" spans="1:5" ht="204" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C35">
@@ -1405,11 +1397,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="4" t="s">
+    <row r="36" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C36">
@@ -1422,11 +1414,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="4" t="s">
+    <row r="37" spans="1:5" ht="289" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C37">
@@ -1444,22 +1436,6 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66C9692C-0347-2F43-9298-96FD60107D90}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>